<commit_message>
Getting Started with the Task Bot Package 09-08-2025:
</commit_message>
<xml_diff>
--- a/Automation Developer Career Quest - Accelerate Phase/Supply Chain Management/StateAssignments.xlsx
+++ b/Automation Developer Career Quest - Accelerate Phase/Supply Chain Management/StateAssignments.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ashish\Automation Anywhere\AA-Solution-Architect-and-Developer\Automation Developer Career Quest - Accelerate Phase\Supply Chain Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213D721A-594B-4159-8188-2626DB1F7D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7317B779-CE46-4B86-86C0-F3DE33C31A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4380BAF2-1F84-46F9-88C7-28B7E57FDE4B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4380BAF2-1F84-46F9-88C7-28B7E57FDE4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -215,8 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -281,7 +280,9 @@
       </font>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{02A20C62-639A-4DC9-A7F6-774DA20037EE}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -297,7 +298,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5F5EC9F-2B9F-45EF-889D-7EF40FAE2BFA}" name="Table1" displayName="Table1" ref="A1:B52" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:B52" xr:uid="{885438B2-97BD-45E4-B86A-AFF9FADFAD0A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B52">
-    <sortCondition ref="A1:A52"/>
+    <sortCondition ref="B2:B52"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{912A36AE-C3AD-4693-9187-BDAE301CE4E3}" name="State"/>
@@ -607,12 +608,12 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.28515625"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -624,411 +625,411 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B42" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s" s="0">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B43" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s" s="0">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B44" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s" s="0">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s" s="0">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s" s="0">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>19</v>
       </c>
-      <c r="B23" t="s" s="0">
+      <c r="B46" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s" s="0">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s" s="0">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s" s="0">
+      <c r="B47" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="B29" t="s" s="0">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s" s="0">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>34</v>
       </c>
-      <c r="B30" t="s" s="0">
+      <c r="B48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="B31" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s" s="0">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>29</v>
       </c>
-      <c r="B32" t="s" s="0">
+      <c r="B49" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="B33" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="B34" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="B35" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="B36" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s" s="0">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s" s="0">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="B43" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s" s="0">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>42</v>
       </c>
-      <c r="B44" t="s" s="0">
+      <c r="B50" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s" s="0">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s" s="0">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>46</v>
       </c>
-      <c r="B47" t="s" s="0">
+      <c r="B51" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B48" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="B49" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s" s="0">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>48</v>
       </c>
-      <c r="B51" t="s" s="0">
+      <c r="B52" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="B52" t="s" s="0">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1040,18 +1041,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1272,18 +1273,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0DF80B-25AB-4B1F-B60A-246B0311BC14}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D060AA8C-26C8-480B-898F-C6958E03794D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D060AA8C-26C8-480B-898F-C6958E03794D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0DF80B-25AB-4B1F-B60A-246B0311BC14}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>